<commit_message>
Added tech field to database
</commit_message>
<xml_diff>
--- a/data/Literature_Review.xlsx
+++ b/data/Literature_Review.xlsx
@@ -13,8 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
-    <sheet name="Results" sheetId="2" r:id="rId2"/>
-    <sheet name="Study_Meta" sheetId="3" r:id="rId3"/>
+    <sheet name="Study_Meta" sheetId="3" r:id="rId2"/>
+    <sheet name="Results" sheetId="2" r:id="rId3"/>
     <sheet name="Results_Meta" sheetId="4" r:id="rId4"/>
     <sheet name="AnalysisSum_Meta" sheetId="5" r:id="rId5"/>
     <sheet name="AnalysisTests_Meta" sheetId="6" r:id="rId6"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="170">
   <si>
     <t>studyID</t>
   </si>
@@ -109,9 +109,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>Difficult because compared between labs; only recorded between-reader internal lab results</t>
   </si>
   <si>
@@ -382,9 +379,6 @@
     <t>Whether (TRUE) or not (FALSE) checked for systematic bias among readers</t>
   </si>
   <si>
-    <t>Whether (TRUE) or not (FALSE) checked for a relationship between the precision metric and age.</t>
-  </si>
-  <si>
     <t>agemin</t>
   </si>
   <si>
@@ -533,6 +527,18 @@
   </si>
   <si>
     <t>APE2</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>Ogle</t>
+  </si>
+  <si>
+    <t>Who deciphered the data</t>
+  </si>
+  <si>
+    <t>Whether (TRUE) or not (FALSE) checked for a relationship between the precision metric and age</t>
   </si>
 </sst>
 </file>
@@ -862,7 +868,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,18 +896,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>2005</v>
@@ -919,21 +925,21 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>1992</v>
       </c>
       <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -944,16 +950,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>1992</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -964,13 +970,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>2004</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -984,7 +990,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>1999</v>
@@ -993,7 +999,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1004,7 +1010,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>2011</v>
@@ -1013,7 +1019,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1024,7 +1030,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>1994</v>
@@ -1033,7 +1039,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1044,13 +1050,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>1987</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -1062,21 +1068,21 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>1989</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -1085,12 +1091,12 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B11">
         <v>2017</v>
@@ -1099,7 +1105,7 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1110,7 +1116,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12">
         <v>2018</v>
@@ -1119,7 +1125,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1127,7 +1133,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B13">
         <v>2011</v>
@@ -1136,7 +1142,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1155,10 +1161,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z24"/>
+  <sheetViews>
+    <sheetView topLeftCell="V1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3:Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,10 +1275,11 @@
     <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5546875" customWidth="1"/>
+    <col min="26" max="26" width="29.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1215,22 +1305,22 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>10</v>
@@ -1239,22 +1329,22 @@
         <v>11</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>14</v>
@@ -1263,12 +1353,15 @@
         <v>15</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1277,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -1331,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="V2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W2" t="b">
         <v>0</v>
@@ -1340,12 +1433,15 @@
         <v>25</v>
       </c>
       <c r="Y2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1354,7 +1450,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -1408,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="V3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W3" t="b">
         <v>0</v>
@@ -1417,12 +1513,15 @@
         <v>25</v>
       </c>
       <c r="Y3" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -1431,7 +1530,7 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -1485,7 +1584,7 @@
         <v>1</v>
       </c>
       <c r="V4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W4" t="b">
         <v>0</v>
@@ -1494,12 +1593,15 @@
         <v>25</v>
       </c>
       <c r="Y4" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1508,7 +1610,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -1562,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="V5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W5" t="b">
         <v>0</v>
@@ -1571,21 +1673,24 @@
         <v>25</v>
       </c>
       <c r="Y5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -1647,19 +1752,22 @@
       <c r="X6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -1721,19 +1829,22 @@
       <c r="X7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -1793,30 +1904,33 @@
         <v>1</v>
       </c>
       <c r="X8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z8" t="s">
         <v>45</v>
       </c>
-      <c r="Y8" t="s">
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -1873,27 +1987,30 @@
         <v>25</v>
       </c>
       <c r="Y9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -1950,21 +2067,24 @@
         <v>25</v>
       </c>
       <c r="Y10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -2026,19 +2146,22 @@
       <c r="X11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -2092,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="V12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W12" t="b">
         <v>0</v>
@@ -2101,15 +2224,18 @@
         <v>25</v>
       </c>
       <c r="Y12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -2118,7 +2244,7 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
         <v>23</v>
@@ -2169,7 +2295,7 @@
         <v>1</v>
       </c>
       <c r="V13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W13" t="b">
         <v>0</v>
@@ -2177,25 +2303,28 @@
       <c r="X13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -2252,27 +2381,30 @@
         <v>25</v>
       </c>
       <c r="Y14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -2329,27 +2461,30 @@
         <v>25</v>
       </c>
       <c r="Y15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -2406,15 +2541,18 @@
         <v>25</v>
       </c>
       <c r="Y16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
@@ -2483,15 +2621,18 @@
         <v>25</v>
       </c>
       <c r="Y17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -2551,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="V18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W18" t="s">
         <v>25</v>
@@ -2559,13 +2700,16 @@
       <c r="X18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -2625,7 +2769,7 @@
         <v>1</v>
       </c>
       <c r="V19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W19" t="s">
         <v>25</v>
@@ -2633,19 +2777,22 @@
       <c r="X19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>22</v>
@@ -2699,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="V20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
@@ -2707,22 +2854,25 @@
       <c r="X20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
         <v>134</v>
-      </c>
-      <c r="C21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" t="s">
-        <v>136</v>
       </c>
       <c r="F21" t="s">
         <v>23</v>
@@ -2781,22 +2931,25 @@
       <c r="X21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
         <v>137</v>
-      </c>
-      <c r="B22" t="s">
-        <v>139</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
         <v>23</v>
@@ -2844,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="V22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W22" t="b">
         <v>0</v>
@@ -2852,19 +3005,22 @@
       <c r="X22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" t="s">
         <v>137</v>
       </c>
-      <c r="B23" t="s">
-        <v>139</v>
-      </c>
       <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" t="s">
         <v>140</v>
-      </c>
-      <c r="D23" t="s">
-        <v>142</v>
       </c>
       <c r="E23" t="s">
         <v>22</v>
@@ -2915,7 +3071,7 @@
         <v>1</v>
       </c>
       <c r="V23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W23" t="b">
         <v>0</v>
@@ -2923,22 +3079,25 @@
       <c r="X23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Y23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" t="s">
         <v>137</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
         <v>139</v>
-      </c>
-      <c r="C24" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" t="s">
-        <v>141</v>
       </c>
       <c r="F24" t="s">
         <v>23</v>
@@ -2986,13 +3145,16 @@
         <v>1</v>
       </c>
       <c r="V24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W24" t="b">
         <v>0</v>
       </c>
       <c r="X24" t="s">
         <v>25</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3003,95 +3165,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3103,13 +3182,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3117,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3125,10 +3204,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3136,10 +3215,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3147,10 +3226,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3158,10 +3237,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3169,10 +3248,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3180,7 +3259,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -3188,55 +3267,55 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
         <v>95</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3244,7 +3323,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -3252,15 +3331,15 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3268,23 +3347,23 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -3292,18 +3371,18 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
         <v>111</v>
-      </c>
-      <c r="C23" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -3311,7 +3390,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -3319,18 +3398,26 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>104</v>
+      <c r="B27" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3355,13 +3442,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3369,7 +3456,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3377,10 +3464,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3388,10 +3475,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3399,10 +3486,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3410,10 +3497,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3421,10 +3508,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3432,7 +3519,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -3440,66 +3527,66 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3507,7 +3594,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3515,15 +3602,15 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3531,23 +3618,23 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3560,7 +3647,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3572,13 +3659,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3586,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3594,10 +3681,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3605,10 +3692,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3616,10 +3703,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3627,10 +3714,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3638,90 +3725,90 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After Josh's Initial review of database
</commit_message>
<xml_diff>
--- a/data/Literature_Review.xlsx
+++ b/data/Literature_Review.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaWork\Research\AgePrecision\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\JFL\Documents\Northland\NRS Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="AnalysisSum_Meta" sheetId="5" r:id="rId5"/>
     <sheet name="AnalysisTests_Meta" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="181">
   <si>
     <t>studyID</t>
   </si>
@@ -539,12 +539,45 @@
   </si>
   <si>
     <t>Whether (TRUE) or not (FALSE) checked for a relationship between the precision metric and age</t>
+  </si>
+  <si>
+    <t>adams_age_2014</t>
+  </si>
+  <si>
+    <t>Blackfin Tuna</t>
+  </si>
+  <si>
+    <t>Little Tunny</t>
+  </si>
+  <si>
+    <t>Skipjack Tuna</t>
+  </si>
+  <si>
+    <t>Lyons</t>
+  </si>
+  <si>
+    <t>Chain Pickerel</t>
+  </si>
+  <si>
+    <t>pelvic</t>
+  </si>
+  <si>
+    <t>anal</t>
+  </si>
+  <si>
+    <t>cleithra</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -582,9 +615,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,18 +905,18 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -905,7 +939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -928,7 +962,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -948,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -968,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -988,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1008,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1028,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1048,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -1071,7 +1105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -1094,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -1114,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -1131,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1167,12 +1201,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -1180,7 +1214,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1188,7 +1222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1196,7 +1230,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1204,7 +1238,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1212,7 +1246,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1220,7 +1254,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1228,7 +1262,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1244,42 +1278,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.21875" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5546875" customWidth="1"/>
-    <col min="26" max="26" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" customWidth="1"/>
+    <col min="26" max="26" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1359,14 +1393,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
@@ -1376,22 +1410,22 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>300</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>40</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2">
+        <v>207</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2">
+        <v>57</v>
       </c>
       <c r="L2" t="s">
         <v>25</v>
@@ -1399,8 +1433,8 @@
       <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="N2">
-        <v>2.5</v>
+      <c r="N2" t="s">
+        <v>25</v>
       </c>
       <c r="O2" t="s">
         <v>25</v>
@@ -1421,10 +1455,10 @@
         <v>25</v>
       </c>
       <c r="U2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="W2" t="b">
         <v>0</v>
@@ -1432,19 +1466,16 @@
       <c r="X2" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+      <c r="Y2" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1456,22 +1487,22 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>300</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>40</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2">
+        <v>203</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2">
+        <v>63</v>
       </c>
       <c r="L3" t="s">
         <v>25</v>
@@ -1479,8 +1510,8 @@
       <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="N3">
-        <v>3.89</v>
+      <c r="N3" t="s">
+        <v>25</v>
       </c>
       <c r="O3" t="s">
         <v>25</v>
@@ -1501,10 +1532,10 @@
         <v>25</v>
       </c>
       <c r="U3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="W3" t="b">
         <v>0</v>
@@ -1512,19 +1543,16 @@
       <c r="X3" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
+      <c r="Y3" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -1536,22 +1564,22 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2">
+        <v>76</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2">
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>25</v>
@@ -1559,8 +1587,8 @@
       <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="N4">
-        <v>5.0199999999999996</v>
+      <c r="N4" t="s">
+        <v>25</v>
       </c>
       <c r="O4" t="s">
         <v>25</v>
@@ -1581,10 +1609,10 @@
         <v>25</v>
       </c>
       <c r="U4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="W4" t="b">
         <v>0</v>
@@ -1592,14 +1620,11 @@
       <c r="X4" t="s">
         <v>25</v>
       </c>
-      <c r="Y4" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y4" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1619,7 +1644,7 @@
         <v>23</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>300</v>
@@ -1640,7 +1665,7 @@
         <v>25</v>
       </c>
       <c r="N5">
-        <v>11.11</v>
+        <v>2.5</v>
       </c>
       <c r="O5" t="s">
         <v>25</v>
@@ -1676,15 +1701,15 @@
         <v>167</v>
       </c>
       <c r="Z5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -1702,13 +1727,13 @@
         <v>4</v>
       </c>
       <c r="H6">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
         <v>25</v>
@@ -1720,7 +1745,7 @@
         <v>25</v>
       </c>
       <c r="N6">
-        <v>5.4</v>
+        <v>3.89</v>
       </c>
       <c r="O6" t="s">
         <v>25</v>
@@ -1741,10 +1766,10 @@
         <v>25</v>
       </c>
       <c r="U6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="W6" t="b">
         <v>0</v>
@@ -1755,13 +1780,16 @@
       <c r="Y6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1776,16 +1804,16 @@
         <v>23</v>
       </c>
       <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>300</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
         <v>25</v>
@@ -1797,7 +1825,7 @@
         <v>25</v>
       </c>
       <c r="N7">
-        <v>5.6</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="O7" t="s">
         <v>25</v>
@@ -1818,10 +1846,10 @@
         <v>25</v>
       </c>
       <c r="U7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="W7" t="b">
         <v>0</v>
@@ -1832,16 +1860,19 @@
       <c r="Y7" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>60</v>
@@ -1853,16 +1884,16 @@
         <v>23</v>
       </c>
       <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>300</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
         <v>25</v>
@@ -1873,8 +1904,8 @@
       <c r="M8" t="s">
         <v>25</v>
       </c>
-      <c r="N8" t="s">
-        <v>25</v>
+      <c r="N8">
+        <v>11.11</v>
       </c>
       <c r="O8" t="s">
         <v>25</v>
@@ -1895,30 +1926,30 @@
         <v>25</v>
       </c>
       <c r="U8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="W8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="Y8" t="s">
         <v>167</v>
       </c>
       <c r="Z8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -1930,19 +1961,19 @@
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>178</v>
+        <v>266</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="K9" t="s">
         <v>25</v>
@@ -1954,7 +1985,7 @@
         <v>25</v>
       </c>
       <c r="N9">
-        <v>6</v>
+        <v>5.4</v>
       </c>
       <c r="O9" t="s">
         <v>25</v>
@@ -1971,8 +2002,8 @@
       <c r="S9" t="s">
         <v>25</v>
       </c>
-      <c r="T9">
-        <v>6</v>
+      <c r="T9" t="s">
+        <v>25</v>
       </c>
       <c r="U9" t="b">
         <v>0</v>
@@ -1989,16 +2020,13 @@
       <c r="Y9" t="s">
         <v>167</v>
       </c>
-      <c r="Z9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -2010,19 +2038,19 @@
         <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>178</v>
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="K10" t="s">
         <v>25</v>
@@ -2034,7 +2062,7 @@
         <v>25</v>
       </c>
       <c r="N10">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="O10" t="s">
         <v>25</v>
@@ -2051,8 +2079,8 @@
       <c r="S10" t="s">
         <v>25</v>
       </c>
-      <c r="T10">
-        <v>10</v>
+      <c r="T10" t="s">
+        <v>25</v>
       </c>
       <c r="U10" t="b">
         <v>0</v>
@@ -2069,19 +2097,16 @@
       <c r="Y10" t="s">
         <v>167</v>
       </c>
-      <c r="Z10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>60</v>
@@ -2093,28 +2118,28 @@
         <v>23</v>
       </c>
       <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>178</v>
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J11">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="K11" t="s">
         <v>25</v>
       </c>
-      <c r="L11">
-        <v>43</v>
-      </c>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>6.3</v>
+      <c r="L11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" t="s">
+        <v>25</v>
       </c>
       <c r="O11" t="s">
         <v>25</v>
@@ -2141,57 +2166,60 @@
         <v>25</v>
       </c>
       <c r="W11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="Y11" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12">
-        <v>3397</v>
+        <v>178</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>16</v>
-      </c>
-      <c r="K12">
-        <v>68</v>
-      </c>
-      <c r="L12">
-        <v>97</v>
-      </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12">
+        <v>6</v>
       </c>
       <c r="O12" t="s">
         <v>25</v>
@@ -2208,14 +2236,14 @@
       <c r="S12" t="s">
         <v>25</v>
       </c>
-      <c r="T12" t="s">
-        <v>25</v>
+      <c r="T12">
+        <v>6</v>
       </c>
       <c r="U12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="W12" t="b">
         <v>0</v>
@@ -2227,51 +2255,51 @@
         <v>167</v>
       </c>
       <c r="Z12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13">
-        <v>603</v>
+        <v>178</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>16</v>
-      </c>
-      <c r="K13">
-        <v>78</v>
-      </c>
-      <c r="L13">
-        <v>97</v>
-      </c>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="K13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13">
+        <v>6</v>
       </c>
       <c r="O13" t="s">
         <v>25</v>
@@ -2288,14 +2316,14 @@
       <c r="S13" t="s">
         <v>25</v>
       </c>
-      <c r="T13" t="s">
-        <v>25</v>
+      <c r="T13">
+        <v>10</v>
       </c>
       <c r="U13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="W13" t="b">
         <v>0</v>
@@ -2306,13 +2334,16 @@
       <c r="Y13" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -2324,31 +2355,31 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="H14">
-        <v>1967</v>
+        <v>178</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
-        <v>8</v>
-      </c>
-      <c r="K14">
-        <v>99.5</v>
+        <v>72</v>
+      </c>
+      <c r="K14" t="s">
+        <v>25</v>
       </c>
       <c r="L14">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="M14" t="b">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>6.3</v>
       </c>
       <c r="O14" t="s">
         <v>25</v>
@@ -2383,49 +2414,46 @@
       <c r="Y14" t="s">
         <v>167</v>
       </c>
-      <c r="Z14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15">
-        <v>1967</v>
+        <v>3397</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K15">
-        <v>99.3</v>
+        <v>68</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" t="s">
         <v>25</v>
@@ -2449,10 +2477,10 @@
         <v>25</v>
       </c>
       <c r="U15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="W15" t="b">
         <v>0</v>
@@ -2464,48 +2492,48 @@
         <v>167</v>
       </c>
       <c r="Z15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
       <c r="H16">
-        <v>1967</v>
+        <v>603</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K16">
-        <v>99.2</v>
+        <v>78</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" t="s">
         <v>25</v>
@@ -2529,10 +2557,10 @@
         <v>25</v>
       </c>
       <c r="U16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="W16" t="b">
         <v>0</v>
@@ -2543,52 +2571,49 @@
       <c r="Y16" t="s">
         <v>167</v>
       </c>
-      <c r="Z16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
         <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>1967</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>25</v>
-      </c>
-      <c r="K17" t="s">
-        <v>25</v>
-      </c>
-      <c r="L17" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" t="s">
-        <v>25</v>
-      </c>
-      <c r="N17">
-        <v>11.2</v>
+        <v>8</v>
+      </c>
+      <c r="K17">
+        <v>99.5</v>
+      </c>
+      <c r="L17">
+        <v>100</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>25</v>
       </c>
       <c r="O17" t="s">
         <v>25</v>
@@ -2608,14 +2633,14 @@
       <c r="T17" t="s">
         <v>25</v>
       </c>
-      <c r="U17" t="s">
-        <v>25</v>
+      <c r="U17" t="b">
+        <v>0</v>
       </c>
       <c r="V17" t="s">
         <v>25</v>
       </c>
-      <c r="W17" t="s">
-        <v>25</v>
+      <c r="W17" t="b">
+        <v>0</v>
       </c>
       <c r="X17" t="s">
         <v>25</v>
@@ -2624,51 +2649,51 @@
         <v>167</v>
       </c>
       <c r="Z17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
-      <c r="H18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" t="s">
-        <v>25</v>
+      <c r="H18">
+        <v>1967</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>21</v>
-      </c>
-      <c r="K18" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="K18">
+        <v>99.3</v>
       </c>
       <c r="L18">
-        <v>65</v>
-      </c>
-      <c r="M18" t="s">
-        <v>25</v>
-      </c>
-      <c r="N18">
-        <v>4.7</v>
+        <v>100</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>25</v>
       </c>
       <c r="O18" t="s">
         <v>25</v>
@@ -2689,13 +2714,13 @@
         <v>25</v>
       </c>
       <c r="U18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" t="s">
-        <v>36</v>
-      </c>
-      <c r="W18" t="s">
-        <v>25</v>
+        <v>25</v>
+      </c>
+      <c r="W18" t="b">
+        <v>0</v>
       </c>
       <c r="X18" t="s">
         <v>25</v>
@@ -2703,49 +2728,52 @@
       <c r="Y18" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" t="s">
-        <v>25</v>
+      <c r="H19">
+        <v>1967</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>13</v>
-      </c>
-      <c r="K19" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>99.2</v>
       </c>
       <c r="L19">
-        <v>95</v>
-      </c>
-      <c r="M19" t="s">
-        <v>25</v>
-      </c>
-      <c r="N19">
-        <v>3.1</v>
+        <v>100</v>
+      </c>
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>25</v>
       </c>
       <c r="O19" t="s">
         <v>25</v>
@@ -2766,13 +2794,13 @@
         <v>25</v>
       </c>
       <c r="U19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" t="s">
-        <v>36</v>
-      </c>
-      <c r="W19" t="s">
-        <v>25</v>
+        <v>25</v>
+      </c>
+      <c r="W19" t="b">
+        <v>0</v>
       </c>
       <c r="X19" t="s">
         <v>25</v>
@@ -2780,19 +2808,22 @@
       <c r="Y19" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="E20" t="s">
         <v>22</v>
@@ -2801,52 +2832,25 @@
         <v>23</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20">
-        <v>266</v>
-      </c>
-      <c r="I20">
-        <v>4</v>
-      </c>
-      <c r="J20">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="K20">
-        <v>72.599999999999994</v>
+        <v>9.52</v>
       </c>
       <c r="L20">
-        <v>97</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="M20" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>2.8</v>
-      </c>
-      <c r="O20" t="s">
-        <v>25</v>
-      </c>
-      <c r="P20" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>25</v>
-      </c>
-      <c r="R20" t="s">
-        <v>25</v>
-      </c>
-      <c r="S20" t="s">
-        <v>25</v>
-      </c>
-      <c r="T20" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="U20" t="b">
         <v>1</v>
       </c>
       <c r="V20" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
@@ -2855,75 +2859,48 @@
         <v>25</v>
       </c>
       <c r="Y20" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="F21" t="s">
         <v>23</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21">
-        <v>62</v>
-      </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
-      <c r="J21">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="K21">
-        <v>46.8</v>
+        <v>19.05</v>
       </c>
       <c r="L21">
-        <v>87.1</v>
+        <v>76.98</v>
       </c>
       <c r="M21" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="O21" t="s">
-        <v>25</v>
-      </c>
-      <c r="P21" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>25</v>
-      </c>
-      <c r="R21" t="s">
-        <v>25</v>
-      </c>
-      <c r="S21" t="s">
-        <v>25</v>
-      </c>
-      <c r="T21" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="U21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="W21" t="b">
         <v>0</v>
@@ -2932,72 +2909,48 @@
         <v>25</v>
       </c>
       <c r="Y21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="E22" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
         <v>23</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H22">
-        <v>151</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="K22">
-        <v>62.3</v>
+        <v>19.05</v>
       </c>
       <c r="L22">
-        <v>94</v>
+        <v>82.14</v>
       </c>
       <c r="M22" t="b">
         <v>1</v>
       </c>
-      <c r="O22">
-        <v>4.7</v>
-      </c>
-      <c r="P22" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>25</v>
-      </c>
-      <c r="R22" t="s">
-        <v>25</v>
-      </c>
-      <c r="S22" t="s">
-        <v>25</v>
-      </c>
-      <c r="T22" t="s">
-        <v>25</v>
-      </c>
       <c r="U22" t="b">
         <v>1</v>
       </c>
       <c r="V22" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="W22" t="b">
         <v>0</v>
@@ -3006,21 +2959,21 @@
         <v>25</v>
       </c>
       <c r="Y22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
         <v>138</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="E23" t="s">
         <v>22</v>
@@ -3029,49 +2982,25 @@
         <v>23</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H23">
-        <v>151</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="K23">
-        <v>56.3</v>
+        <v>9.52</v>
       </c>
       <c r="L23">
-        <v>88.7</v>
+        <v>76.98</v>
       </c>
       <c r="M23" t="b">
         <v>1</v>
       </c>
-      <c r="O23">
-        <v>12.1</v>
-      </c>
-      <c r="P23" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>25</v>
-      </c>
-      <c r="R23" t="s">
-        <v>25</v>
-      </c>
-      <c r="S23" t="s">
-        <v>25</v>
-      </c>
-      <c r="T23" t="s">
-        <v>25</v>
-      </c>
       <c r="U23" t="b">
         <v>1</v>
       </c>
       <c r="V23" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="W23" t="b">
         <v>0</v>
@@ -3080,21 +3009,21 @@
         <v>25</v>
       </c>
       <c r="Y23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="C24" t="s">
         <v>133</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>140</v>
       </c>
       <c r="E24" t="s">
         <v>139</v>
@@ -3103,65 +3032,807 @@
         <v>23</v>
       </c>
       <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>42</v>
+      </c>
+      <c r="K24">
+        <v>11.9</v>
+      </c>
+      <c r="L24">
+        <v>83.73</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U24" t="b">
+        <v>1</v>
+      </c>
+      <c r="V24" t="s">
+        <v>35</v>
+      </c>
+      <c r="W24" t="b">
+        <v>0</v>
+      </c>
+      <c r="X24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>42</v>
+      </c>
+      <c r="K25">
+        <v>21.43</v>
+      </c>
+      <c r="L25">
+        <v>88.1</v>
+      </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
+      <c r="U25" t="b">
+        <v>1</v>
+      </c>
+      <c r="V25" t="s">
+        <v>35</v>
+      </c>
+      <c r="W25" t="b">
+        <v>0</v>
+      </c>
+      <c r="X25" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>42</v>
+      </c>
+      <c r="K26">
+        <v>23.81</v>
+      </c>
+      <c r="L26">
+        <v>78.569999999999993</v>
+      </c>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
+      <c r="U26" t="b">
+        <v>1</v>
+      </c>
+      <c r="V26" t="s">
+        <v>35</v>
+      </c>
+      <c r="W26" t="b">
+        <v>0</v>
+      </c>
+      <c r="X26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>42</v>
+      </c>
+      <c r="K27">
+        <v>40.479999999999997</v>
+      </c>
+      <c r="L27">
+        <v>97.22</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U27" t="b">
+        <v>1</v>
+      </c>
+      <c r="V27" t="s">
+        <v>35</v>
+      </c>
+      <c r="W27" t="b">
+        <v>0</v>
+      </c>
+      <c r="X27" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28">
+        <v>25</v>
+      </c>
+      <c r="K28" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28">
+        <v>11.2</v>
+      </c>
+      <c r="O28" t="s">
+        <v>25</v>
+      </c>
+      <c r="P28" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" t="s">
+        <v>25</v>
+      </c>
+      <c r="S28" t="s">
+        <v>25</v>
+      </c>
+      <c r="T28" t="s">
+        <v>25</v>
+      </c>
+      <c r="U28" t="s">
+        <v>25</v>
+      </c>
+      <c r="V28" t="s">
+        <v>25</v>
+      </c>
+      <c r="W28" t="s">
+        <v>25</v>
+      </c>
+      <c r="X28" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29">
         <v>2</v>
       </c>
-      <c r="H24">
+      <c r="H29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29">
+        <v>21</v>
+      </c>
+      <c r="K29" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29">
+        <v>65</v>
+      </c>
+      <c r="M29" t="s">
+        <v>25</v>
+      </c>
+      <c r="N29">
+        <v>4.7</v>
+      </c>
+      <c r="O29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P29" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>25</v>
+      </c>
+      <c r="R29" t="s">
+        <v>25</v>
+      </c>
+      <c r="S29" t="s">
+        <v>25</v>
+      </c>
+      <c r="T29" t="s">
+        <v>25</v>
+      </c>
+      <c r="U29" t="b">
+        <v>1</v>
+      </c>
+      <c r="V29" t="s">
+        <v>36</v>
+      </c>
+      <c r="W29" t="s">
+        <v>25</v>
+      </c>
+      <c r="X29" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30">
+        <v>13</v>
+      </c>
+      <c r="K30" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30">
+        <v>95</v>
+      </c>
+      <c r="M30" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30">
+        <v>3.1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>25</v>
+      </c>
+      <c r="P30" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>25</v>
+      </c>
+      <c r="R30" t="s">
+        <v>25</v>
+      </c>
+      <c r="S30" t="s">
+        <v>25</v>
+      </c>
+      <c r="T30" t="s">
+        <v>25</v>
+      </c>
+      <c r="U30" t="b">
+        <v>1</v>
+      </c>
+      <c r="V30" t="s">
+        <v>36</v>
+      </c>
+      <c r="W30" t="s">
+        <v>25</v>
+      </c>
+      <c r="X30" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>266</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <v>20</v>
+      </c>
+      <c r="K31">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="L31">
+        <v>97</v>
+      </c>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>2.8</v>
+      </c>
+      <c r="O31" t="s">
+        <v>25</v>
+      </c>
+      <c r="P31" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>25</v>
+      </c>
+      <c r="R31" t="s">
+        <v>25</v>
+      </c>
+      <c r="S31" t="s">
+        <v>25</v>
+      </c>
+      <c r="T31" t="s">
+        <v>25</v>
+      </c>
+      <c r="U31" t="b">
+        <v>1</v>
+      </c>
+      <c r="V31" t="s">
+        <v>162</v>
+      </c>
+      <c r="W31" t="b">
+        <v>0</v>
+      </c>
+      <c r="X31" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>62</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>8</v>
+      </c>
+      <c r="K32">
+        <v>46.8</v>
+      </c>
+      <c r="L32">
+        <v>87.1</v>
+      </c>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="O32" t="s">
+        <v>25</v>
+      </c>
+      <c r="P32" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>25</v>
+      </c>
+      <c r="R32" t="s">
+        <v>25</v>
+      </c>
+      <c r="S32" t="s">
+        <v>25</v>
+      </c>
+      <c r="T32" t="s">
+        <v>25</v>
+      </c>
+      <c r="U32" t="b">
+        <v>0</v>
+      </c>
+      <c r="V32" t="s">
+        <v>25</v>
+      </c>
+      <c r="W32" t="b">
+        <v>0</v>
+      </c>
+      <c r="X32" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
         <v>151</v>
       </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>23</v>
+      </c>
+      <c r="K33">
+        <v>62.3</v>
+      </c>
+      <c r="L33">
+        <v>94</v>
+      </c>
+      <c r="M33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>4.7</v>
+      </c>
+      <c r="P33" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>25</v>
+      </c>
+      <c r="R33" t="s">
+        <v>25</v>
+      </c>
+      <c r="S33" t="s">
+        <v>25</v>
+      </c>
+      <c r="T33" t="s">
+        <v>25</v>
+      </c>
+      <c r="U33" t="b">
+        <v>1</v>
+      </c>
+      <c r="V33" t="s">
+        <v>162</v>
+      </c>
+      <c r="W33" t="b">
+        <v>0</v>
+      </c>
+      <c r="X33" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>151</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="K34">
+        <v>56.3</v>
+      </c>
+      <c r="L34">
+        <v>88.7</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>12.1</v>
+      </c>
+      <c r="P34" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>25</v>
+      </c>
+      <c r="R34" t="s">
+        <v>25</v>
+      </c>
+      <c r="S34" t="s">
+        <v>25</v>
+      </c>
+      <c r="T34" t="s">
+        <v>25</v>
+      </c>
+      <c r="U34" t="b">
+        <v>1</v>
+      </c>
+      <c r="V34" t="s">
+        <v>162</v>
+      </c>
+      <c r="W34" t="b">
+        <v>0</v>
+      </c>
+      <c r="X34" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>151</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
         <v>16</v>
       </c>
-      <c r="K24">
+      <c r="K35">
         <v>45.7</v>
       </c>
-      <c r="L24">
+      <c r="L35">
         <v>75.5</v>
       </c>
-      <c r="M24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O24">
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
+      <c r="O35">
         <v>7.4</v>
       </c>
-      <c r="P24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>25</v>
-      </c>
-      <c r="R24" t="s">
-        <v>25</v>
-      </c>
-      <c r="S24" t="s">
-        <v>25</v>
-      </c>
-      <c r="T24" t="s">
-        <v>25</v>
-      </c>
-      <c r="U24" t="b">
-        <v>1</v>
-      </c>
-      <c r="V24" t="s">
+      <c r="P35" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>25</v>
+      </c>
+      <c r="R35" t="s">
+        <v>25</v>
+      </c>
+      <c r="S35" t="s">
+        <v>25</v>
+      </c>
+      <c r="T35" t="s">
+        <v>25</v>
+      </c>
+      <c r="U35" t="b">
+        <v>1</v>
+      </c>
+      <c r="V35" t="s">
         <v>162</v>
       </c>
-      <c r="W24" t="b">
-        <v>0</v>
-      </c>
-      <c r="X24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y24" t="s">
+      <c r="W35" t="b">
+        <v>0</v>
+      </c>
+      <c r="X35" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y35" t="s">
         <v>167</v>
       </c>
     </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:Y19">
+  <sortState ref="A5:Y30">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3169,18 +3840,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -3191,7 +3862,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3199,7 +3870,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3210,7 +3881,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3221,7 +3892,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3232,7 +3903,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3243,7 +3914,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3254,7 +3925,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3262,7 +3933,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3270,7 +3941,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -3278,7 +3949,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -3286,7 +3957,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -3294,7 +3965,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -3302,7 +3973,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -3310,7 +3981,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -3318,7 +3989,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -3326,7 +3997,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -3334,7 +4005,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>164</v>
       </c>
@@ -3342,7 +4013,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3350,7 +4021,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>165</v>
       </c>
@@ -3358,7 +4029,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3366,7 +4037,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -3374,7 +4045,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -3385,7 +4056,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -3393,7 +4064,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -3404,7 +4075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>166</v>
       </c>
@@ -3412,7 +4083,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3429,18 +4100,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -3451,7 +4122,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3459,7 +4130,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3470,7 +4141,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3481,7 +4152,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3492,7 +4163,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3503,7 +4174,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3514,7 +4185,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3522,7 +4193,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3530,7 +4201,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -3541,7 +4212,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3549,7 +4220,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -3557,7 +4228,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -3565,7 +4236,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -3573,7 +4244,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3581,7 +4252,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3589,7 +4260,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -3597,7 +4268,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -3605,7 +4276,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -3613,7 +4284,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3621,7 +4292,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -3629,7 +4300,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -3646,18 +4317,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -3668,7 +4339,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3676,7 +4347,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3687,7 +4358,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3698,7 +4369,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3709,7 +4380,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3720,7 +4391,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3731,7 +4402,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -3739,7 +4410,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -3747,7 +4418,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -3755,7 +4426,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -3763,7 +4434,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -3771,7 +4442,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -3779,7 +4450,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -3787,7 +4458,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -3795,7 +4466,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -3803,7 +4474,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>151</v>
       </c>

</xml_diff>